<commit_message>
corrected minor label mistakes
</commit_message>
<xml_diff>
--- a/excel_data/coords_xy_edges_verticies.xlsx
+++ b/excel_data/coords_xy_edges_verticies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Nextcloud\Master\Disk_Tiling_Measurements\MADMAX_disk_analysis\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C050DD-2AC8-4D09-8DBE-3922852374DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D8A764-9B77-49F8-87E2-A96CA0E4939E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5CB6071D-5A0D-4933-88AF-6C0C8BC4CBF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{5CB6071D-5A0D-4933-88AF-6C0C8BC4CBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="68">
   <si>
     <t>arm_label</t>
   </si>
@@ -204,6 +204,42 @@
   </si>
   <si>
     <t>vertex</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>h3</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>h5</t>
+  </si>
+  <si>
+    <t>h6</t>
+  </si>
+  <si>
+    <t>h7</t>
+  </si>
+  <si>
+    <t>h8</t>
+  </si>
+  <si>
+    <t>h9</t>
+  </si>
+  <si>
+    <t>h10</t>
+  </si>
+  <si>
+    <t>h11</t>
+  </si>
+  <si>
+    <t>h12</t>
   </si>
 </sst>
 </file>
@@ -299,11 +335,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -324,13 +356,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F0BC9290-4FD2-412D-995E-77626F21D122}" name="Tabelle2" displayName="Tabelle2" ref="A1:D67" totalsRowShown="0">
-  <autoFilter ref="A1:D67" xr:uid="{F0BC9290-4FD2-412D-995E-77626F21D122}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E8B9C32-EB39-486E-9D3A-69ED010B0909}" name="Tabelle1" displayName="Tabelle1" ref="A1:D79" totalsRowShown="0">
+  <autoFilter ref="A1:D79" xr:uid="{1E8B9C32-EB39-486E-9D3A-69ED010B0909}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D4D79E92-90B9-4FEE-A3B7-577D16015D00}" name="arm_label" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{7F3937DC-3768-41BA-B8AB-3153F11A8AB8}" name="arm_type"/>
-    <tableColumn id="3" xr3:uid="{8F1CDF28-D638-4553-8B2B-669971F77680}" name="x"/>
-    <tableColumn id="4" xr3:uid="{982BBD35-5957-406E-AFE4-8636CA992E8B}" name="y"/>
+    <tableColumn id="1" xr3:uid="{B133811A-9490-4CB8-AF33-075C042239DF}" name="arm_label"/>
+    <tableColumn id="2" xr3:uid="{0B942E28-BFB1-41D6-BB34-C0C38DE29721}" name="arm_type"/>
+    <tableColumn id="3" xr3:uid="{36B520B2-3296-4FF4-BB62-72E9BC0EF6FA}" name="x"/>
+    <tableColumn id="4" xr3:uid="{69A33587-36B9-4167-A69E-168EC6C5D580}" name="y"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B490DF-0CB4-4A29-B289-93BF6538B8D3}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,6 +1716,198 @@
         <v>-75.338999999999999</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68">
+        <f>C55</f>
+        <v>-97.877999999999986</v>
+      </c>
+      <c r="D68">
+        <f>D51</f>
+        <v>94.191000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69">
+        <f>C51</f>
+        <v>-32.625999999999998</v>
+      </c>
+      <c r="D69">
+        <f>3*J6-J4</f>
+        <v>131.84899999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70">
+        <f>-C69</f>
+        <v>32.625999999999998</v>
+      </c>
+      <c r="D70">
+        <f>D69</f>
+        <v>131.84899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71">
+        <f>-C68</f>
+        <v>97.877999999999986</v>
+      </c>
+      <c r="D71">
+        <f>D68</f>
+        <v>94.191000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72">
+        <f>4*J5</f>
+        <v>130.50399999999999</v>
+      </c>
+      <c r="D72">
+        <f>J4</f>
+        <v>37.680999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73">
+        <f>C72</f>
+        <v>130.50399999999999</v>
+      </c>
+      <c r="D73">
+        <f>-D72</f>
+        <v>-37.680999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74">
+        <f>C71</f>
+        <v>97.877999999999986</v>
+      </c>
+      <c r="D74">
+        <f>-D71</f>
+        <v>-94.191000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75">
+        <f>C70</f>
+        <v>32.625999999999998</v>
+      </c>
+      <c r="D75">
+        <f>-D70</f>
+        <v>-131.84899999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76">
+        <f>C69</f>
+        <v>-32.625999999999998</v>
+      </c>
+      <c r="D76">
+        <f>-D69</f>
+        <v>-131.84899999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77">
+        <f>-C74</f>
+        <v>-97.877999999999986</v>
+      </c>
+      <c r="D77">
+        <f>D74</f>
+        <v>-94.191000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78">
+        <f>-C73</f>
+        <v>-130.50399999999999</v>
+      </c>
+      <c r="D78">
+        <f>D73</f>
+        <v>-37.680999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79">
+        <f>-C72</f>
+        <v>-130.50399999999999</v>
+      </c>
+      <c r="D79">
+        <f>D72</f>
+        <v>37.680999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1692,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CBDC93-EE51-4D71-A6BA-9B8929A64511}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1994,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>-97.878</v>
+        <v>-97.877999999999986</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2642,6 +2866,174 @@
       </c>
       <c r="D67">
         <v>-75.338999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68">
+        <v>-97.877999999999986</v>
+      </c>
+      <c r="D68">
+        <v>94.191000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69">
+        <v>-32.625999999999998</v>
+      </c>
+      <c r="D69">
+        <v>131.84899999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70">
+        <v>32.625999999999998</v>
+      </c>
+      <c r="D70">
+        <v>131.84899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71">
+        <v>97.877999999999986</v>
+      </c>
+      <c r="D71">
+        <v>94.191000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72">
+        <v>130.50399999999999</v>
+      </c>
+      <c r="D72">
+        <v>37.680999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73">
+        <v>130.50399999999999</v>
+      </c>
+      <c r="D73">
+        <v>-37.680999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74">
+        <v>97.877999999999986</v>
+      </c>
+      <c r="D74">
+        <v>-94.191000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75">
+        <v>32.625999999999998</v>
+      </c>
+      <c r="D75">
+        <v>-131.84899999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76">
+        <v>-32.625999999999998</v>
+      </c>
+      <c r="D76">
+        <v>-131.84899999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77">
+        <v>-97.877999999999986</v>
+      </c>
+      <c r="D77">
+        <v>-94.191000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78">
+        <v>-130.50399999999999</v>
+      </c>
+      <c r="D78">
+        <v>-37.680999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79">
+        <v>-130.50399999999999</v>
+      </c>
+      <c r="D79">
+        <v>37.680999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>